<commit_message>
add test random packing spheres
</commit_message>
<xml_diff>
--- a/Result/Sc/Sum.xlsx
+++ b/Result/Sc/Sum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">SBB-MRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIBB-MRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QIBB-MRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MR-MRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLI-MRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSM-MRT-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSM-MRT-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM-MRT-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM-MRT-B</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -124,41 +156,41 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="K14" activeCellId="1" sqref="J1:J12 K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="n">
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>-2</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>-3</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>-4</v>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +211,7 @@
       <c r="G3" s="1" t="n">
         <v>0.045204333</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.0479838317</v>
       </c>
     </row>
@@ -202,7 +234,7 @@
       <c r="G4" s="1" t="n">
         <v>0.0640125522</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.0614631682</v>
       </c>
     </row>
@@ -229,13 +261,13 @@
         <v>0.0720869451</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.0687818749</v>
+        <v>0.0578070408</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0.0754685303</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.0578070408</v>
+        <v>0.0687818749</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,13 +293,13 @@
         <v>0.0741891209</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>0.0734844452</v>
+        <v>0.0637099542</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>0.0794618253</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>0.0637099542</v>
+        <v>0.0734844452</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,13 +325,13 @@
         <v>0.0749262329</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0.0770220228</v>
+        <v>0.06655892</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>0.0820082695</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0.06655892</v>
+        <v>0.0770220228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,13 +357,13 @@
         <v>0.0755579276</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0804531221</v>
+        <v>0.0685385114</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>0.084367324</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.0685385114</v>
+        <v>0.0804531221</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,13 +389,13 @@
         <v>0.0761283293</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>0.0838341362</v>
+        <v>0.0700618526</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>0.0866312698</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>0.0700618526</v>
+        <v>0.0838341362</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,13 +421,13 @@
         <v>0.0766527021</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0.0871800011</v>
+        <v>0.0713024869</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>0.0888339192</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0.0713024869</v>
+        <v>0.0871800011</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,13 +453,13 @@
         <v>0.0771403229</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>0.090497174</v>
+        <v>0.0723509315</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>0.0909923535</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0723509315</v>
+        <v>0.090497174</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,13 +485,13 @@
         <v>0.0775979651</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>0.093792306</v>
+        <v>0.0732607788</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>0.0931166073</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0732607788</v>
+        <v>0.093792306</v>
       </c>
     </row>
   </sheetData>
@@ -481,13 +513,10 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -509,13 +538,13 @@
         <v>-1</v>
       </c>
       <c r="H1" s="0" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="I1" s="0" t="n">
         <v>-3</v>
       </c>
       <c r="J1" s="0" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,13 +570,13 @@
         <v>0.0702448834</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.0537829994</v>
+        <v>0.0556371669</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>0.0575077397</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.0556371669</v>
+        <v>0.0537829994</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,13 +587,13 @@
         <v>0.0733457607</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>0.0568246233</v>
+        <v>0.0628288517</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>0.0616829893</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>0.0628288517</v>
+        <v>0.0568246233</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,13 +604,13 @@
         <v>0.0753816119</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0.0603235488</v>
+        <v>0.0670222377</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>0.0645796716</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0.0670222377</v>
+        <v>0.0603235488</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,13 +621,13 @@
         <v>0.0776142887</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0645362216</v>
+        <v>0.0705913135</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>0.0682070116</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.0705913135</v>
+        <v>0.0645362216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,13 +638,13 @@
         <v>0.0800905332</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>0.0692743624</v>
+        <v>0.0739843744</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>0.0723616566</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>0.0739843744</v>
+        <v>0.0692743624</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,13 +655,13 @@
         <v>0.0828066458</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0.0744145792</v>
+        <v>0.0773689857</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>0.0769113519</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0.0773689857</v>
+        <v>0.0744145792</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,13 +672,13 @@
         <v>0.0857498527</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>0.079877336</v>
+        <v>0.0808199013</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>0.0817735202</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.0808199013</v>
+        <v>0.079877336</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,13 +689,13 @@
         <v>0.0889078266</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>0.0856101896</v>
+        <v>0.0843748941</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>0.0868966603</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>0.0843748941</v>
+        <v>0.0856101896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>